<commit_message>
fiz uma string de conexão do firebird com o python
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estagioti\Desktop\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71682FFC-D084-49A6-9109-7B697FE52C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E55DD4-7C1F-4E57-B86F-F72431532C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4050" yWindow="3285" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Produto</t>
   </si>
@@ -39,9 +39,6 @@
     <t>macarrão</t>
   </si>
   <si>
-    <t>Gastos</t>
-  </si>
-  <si>
     <t>lentilha</t>
   </si>
   <si>
@@ -49,6 +46,15 @@
   </si>
   <si>
     <t>café</t>
+  </si>
+  <si>
+    <t>Vendas</t>
+  </si>
+  <si>
+    <t>açucar</t>
+  </si>
+  <si>
+    <t>sal</t>
   </si>
 </sst>
 </file>
@@ -387,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,7 +409,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -432,7 +438,7 @@
     </row>
     <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2">
         <v>30</v>
@@ -440,7 +446,7 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2">
         <v>70</v>
@@ -448,15 +454,27 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>